<commit_message>
minor changes for FGI paper
</commit_message>
<xml_diff>
--- a/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_A_FGI_corn.xlsx
+++ b/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_A_FGI_corn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\repository_clones\Bioindustrial-Park\biorefineries\TAL\analyses\full\parameter_distributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CF3AC7-71B8-4640-AC77-C93245E2580F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B759F801-F628-4D45-BD1A-88B9BD02608A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3580" yWindow="2500" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -827,7 +827,7 @@
   <dimension ref="A1:Q51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD25"/>
+      <selection activeCell="B1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>